<commit_message>
Conferência dados DW - FatDev
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_FatDev_DW.xlsx
+++ b/Documentação/Planilhas/Conferencia_FatDev_DW.xlsx
@@ -712,9 +712,6 @@
     <t>É a concatenação dos campos NR_NF_ORIG + DS_SERIE + NR_FILIAL</t>
   </si>
   <si>
-    <t>Quando receber o cancelamento de uma nota, ficará com 1. Sem cancelamento, fica com zeros</t>
-  </si>
-  <si>
     <t>Externo ao LN</t>
   </si>
   <si>
@@ -843,6 +840,9 @@
   </si>
   <si>
     <t>Na aba superior "Expedição", pegar a informação do "Cód da Lista de Casamento"</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna "Status da Fatura". Se for "Cancelar", virá como 1, caso contrário, zero</t>
   </si>
 </sst>
 </file>
@@ -971,7 +971,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -998,33 +998,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1034,64 +1007,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1130,70 +1050,13 @@
     <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1202,16 +1065,46 @@
     <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1517,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:BT39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BO28" sqref="BO28"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX14" sqref="AX14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1580,7 +1473,8 @@
     <col min="55" max="55" width="23.5703125" style="1" customWidth="1"/>
     <col min="56" max="56" width="38.140625" style="1" customWidth="1"/>
     <col min="57" max="57" width="42.5703125" style="1" customWidth="1"/>
-    <col min="58" max="60" width="22.85546875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="45.28515625" style="1" customWidth="1"/>
+    <col min="59" max="60" width="22.85546875" style="1" customWidth="1"/>
     <col min="61" max="61" width="21.42578125" style="1" customWidth="1"/>
     <col min="62" max="62" width="19.5703125" style="1" customWidth="1"/>
     <col min="63" max="67" width="22.85546875" style="1" customWidth="1"/>
@@ -1593,237 +1487,234 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:72" ht="11.25" customHeight="1">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
+      <c r="AR2" s="18"/>
+      <c r="AS2" s="18"/>
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="18"/>
+      <c r="AV2" s="18"/>
+      <c r="AW2" s="18"/>
+      <c r="AX2" s="18"/>
+      <c r="AY2" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="37"/>
-      <c r="AU2" s="37"/>
-      <c r="AV2" s="37"/>
-      <c r="AW2" s="37"/>
-      <c r="AX2" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="AY2" s="27"/>
-      <c r="AZ2" s="27"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
-      <c r="BC2" s="27"/>
-      <c r="BD2" s="28"/>
-      <c r="BE2" s="32" t="s">
-        <v>231</v>
-      </c>
-      <c r="BF2" s="35" t="s">
+      <c r="BG2" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="BH2" s="15"/>
+      <c r="BI2" s="15"/>
+      <c r="BJ2" s="15"/>
+      <c r="BK2" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="BG2" s="35"/>
-      <c r="BH2" s="35"/>
-      <c r="BI2" s="35"/>
-      <c r="BJ2" s="36" t="s">
-        <v>268</v>
-      </c>
-      <c r="BK2" s="36"/>
-      <c r="BL2" s="36"/>
-      <c r="BM2" s="36"/>
-      <c r="BN2" s="36"/>
-      <c r="BO2" s="36"/>
-      <c r="BP2" s="36"/>
-      <c r="BQ2" s="36"/>
-      <c r="BR2" s="36"/>
-      <c r="BS2" s="36"/>
-      <c r="BT2" s="36"/>
+      <c r="BL2" s="17"/>
+      <c r="BM2" s="17"/>
+      <c r="BN2" s="17"/>
+      <c r="BO2" s="17"/>
+      <c r="BP2" s="17"/>
+      <c r="BQ2" s="17"/>
+      <c r="BR2" s="17"/>
+      <c r="BS2" s="17"/>
     </row>
     <row r="3" spans="1:72" ht="11.25" customHeight="1">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37"/>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="37"/>
-      <c r="AO3" s="37"/>
-      <c r="AP3" s="37"/>
-      <c r="AQ3" s="37"/>
-      <c r="AR3" s="37"/>
-      <c r="AS3" s="37"/>
-      <c r="AT3" s="37"/>
-      <c r="AU3" s="37"/>
-      <c r="AV3" s="37"/>
-      <c r="AW3" s="37"/>
-      <c r="AX3" s="29"/>
-      <c r="AY3" s="30"/>
-      <c r="AZ3" s="30"/>
-      <c r="BA3" s="30"/>
-      <c r="BB3" s="30"/>
-      <c r="BC3" s="30"/>
-      <c r="BD3" s="31"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="18"/>
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="18"/>
+      <c r="AM3" s="18"/>
+      <c r="AN3" s="18"/>
+      <c r="AO3" s="18"/>
+      <c r="AP3" s="18"/>
+      <c r="AQ3" s="18"/>
+      <c r="AR3" s="18"/>
+      <c r="AS3" s="18"/>
+      <c r="AT3" s="18"/>
+      <c r="AU3" s="18"/>
+      <c r="AV3" s="18"/>
+      <c r="AW3" s="18"/>
+      <c r="AX3" s="18"/>
+      <c r="AY3" s="32"/>
+      <c r="AZ3" s="32"/>
+      <c r="BA3" s="32"/>
+      <c r="BB3" s="32"/>
+      <c r="BC3" s="32"/>
+      <c r="BD3" s="32"/>
       <c r="BE3" s="32"/>
-      <c r="BF3" s="35"/>
-      <c r="BG3" s="35"/>
-      <c r="BH3" s="35"/>
-      <c r="BI3" s="35"/>
-      <c r="BJ3" s="36"/>
-      <c r="BK3" s="36"/>
-      <c r="BL3" s="36"/>
-      <c r="BM3" s="36"/>
-      <c r="BN3" s="36"/>
-      <c r="BO3" s="36"/>
-      <c r="BP3" s="36"/>
-      <c r="BQ3" s="36"/>
-      <c r="BR3" s="36"/>
-      <c r="BS3" s="36"/>
-      <c r="BT3" s="36"/>
+      <c r="BF3" s="21"/>
+      <c r="BG3" s="15"/>
+      <c r="BH3" s="15"/>
+      <c r="BI3" s="15"/>
+      <c r="BJ3" s="15"/>
+      <c r="BK3" s="17"/>
+      <c r="BL3" s="17"/>
+      <c r="BM3" s="17"/>
+      <c r="BN3" s="17"/>
+      <c r="BO3" s="17"/>
+      <c r="BP3" s="17"/>
+      <c r="BQ3" s="17"/>
+      <c r="BR3" s="17"/>
+      <c r="BS3" s="17"/>
     </row>
     <row r="4" spans="1:72" ht="11.25" customHeight="1">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="37"/>
-      <c r="AD4" s="37"/>
-      <c r="AE4" s="37"/>
-      <c r="AF4" s="37"/>
-      <c r="AG4" s="37"/>
-      <c r="AH4" s="37"/>
-      <c r="AI4" s="37"/>
-      <c r="AJ4" s="37"/>
-      <c r="AK4" s="37"/>
-      <c r="AL4" s="37"/>
-      <c r="AM4" s="37"/>
-      <c r="AN4" s="37"/>
-      <c r="AO4" s="37"/>
-      <c r="AP4" s="37"/>
-      <c r="AQ4" s="37"/>
-      <c r="AR4" s="37"/>
-      <c r="AS4" s="37"/>
-      <c r="AT4" s="37"/>
-      <c r="AU4" s="37"/>
-      <c r="AV4" s="37"/>
-      <c r="AW4" s="37"/>
-      <c r="AX4" s="39"/>
-      <c r="AY4" s="40"/>
-      <c r="AZ4" s="40"/>
-      <c r="BA4" s="40"/>
-      <c r="BB4" s="40"/>
-      <c r="BC4" s="40"/>
-      <c r="BD4" s="41"/>
-      <c r="BE4" s="33"/>
-      <c r="BF4" s="35"/>
-      <c r="BG4" s="35"/>
-      <c r="BH4" s="35"/>
-      <c r="BI4" s="35"/>
-      <c r="BJ4" s="36"/>
-      <c r="BK4" s="36"/>
-      <c r="BL4" s="36"/>
-      <c r="BM4" s="36"/>
-      <c r="BN4" s="36"/>
-      <c r="BO4" s="36"/>
-      <c r="BP4" s="36"/>
-      <c r="BQ4" s="36"/>
-      <c r="BR4" s="36"/>
-      <c r="BS4" s="36"/>
-      <c r="BT4" s="36"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
+      <c r="AN4" s="18"/>
+      <c r="AO4" s="18"/>
+      <c r="AP4" s="18"/>
+      <c r="AQ4" s="18"/>
+      <c r="AR4" s="18"/>
+      <c r="AS4" s="18"/>
+      <c r="AT4" s="18"/>
+      <c r="AU4" s="18"/>
+      <c r="AV4" s="18"/>
+      <c r="AW4" s="18"/>
+      <c r="AX4" s="18"/>
+      <c r="AY4" s="32"/>
+      <c r="AZ4" s="32"/>
+      <c r="BA4" s="32"/>
+      <c r="BB4" s="32"/>
+      <c r="BC4" s="32"/>
+      <c r="BD4" s="32"/>
+      <c r="BE4" s="32"/>
+      <c r="BF4" s="22"/>
+      <c r="BG4" s="15"/>
+      <c r="BH4" s="15"/>
+      <c r="BI4" s="15"/>
+      <c r="BJ4" s="15"/>
+      <c r="BK4" s="17"/>
+      <c r="BL4" s="17"/>
+      <c r="BM4" s="17"/>
+      <c r="BN4" s="17"/>
+      <c r="BO4" s="17"/>
+      <c r="BP4" s="17"/>
+      <c r="BQ4" s="17"/>
+      <c r="BR4" s="17"/>
+      <c r="BS4" s="17"/>
     </row>
     <row r="5" spans="1:72" s="4" customFormat="1" ht="24.75" customHeight="1">
       <c r="A5" s="11" t="s">
@@ -1836,7 +1727,7 @@
         <v>44</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>6</v>
@@ -1857,160 +1748,160 @@
         <v>1</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="M5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="N5" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="O5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="R5" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="S5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="T5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="U5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="V5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="V5" s="11" t="s">
+      <c r="W5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="W5" s="11" t="s">
+      <c r="X5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="X5" s="11" t="s">
+      <c r="Y5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="11" t="s">
+      <c r="Z5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z5" s="11" t="s">
+      <c r="AA5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AA5" s="11" t="s">
+      <c r="AB5" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AB5" s="11" t="s">
+      <c r="AC5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AC5" s="11" t="s">
+      <c r="AD5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="11" t="s">
+      <c r="AE5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AE5" s="11" t="s">
+      <c r="AF5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="11" t="s">
+      <c r="AG5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AG5" s="11" t="s">
+      <c r="AH5" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AH5" s="11" t="s">
+      <c r="AI5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI5" s="11" t="s">
+      <c r="AJ5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ5" s="11" t="s">
+      <c r="AK5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AK5" s="11" t="s">
+      <c r="AL5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AL5" s="11" t="s">
+      <c r="AM5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AM5" s="11" t="s">
+      <c r="AN5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AN5" s="11" t="s">
+      <c r="AO5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AO5" s="11" t="s">
+      <c r="AP5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AP5" s="11" t="s">
+      <c r="AQ5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AQ5" s="11" t="s">
+      <c r="AR5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AR5" s="11" t="s">
+      <c r="AS5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AS5" s="11" t="s">
+      <c r="AT5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AT5" s="11" t="s">
+      <c r="AU5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="AU5" s="11" t="s">
+      <c r="AV5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AV5" s="11" t="s">
+      <c r="AW5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AW5" s="11" t="s">
+      <c r="AX5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AX5" s="11" t="s">
+      <c r="AY5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AY5" s="11" t="s">
+      <c r="AZ5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AZ5" s="11" t="s">
+      <c r="BA5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="BA5" s="11" t="s">
+      <c r="BB5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BB5" s="11" t="s">
+      <c r="BC5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="BC5" s="11" t="s">
+      <c r="BD5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="BD5" s="11" t="s">
+      <c r="BE5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="BE5" s="11" t="s">
+      <c r="BF5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="BF5" s="11" t="s">
+      <c r="BG5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="BG5" s="11" t="s">
+      <c r="BH5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="BH5" s="11" t="s">
+      <c r="BI5" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="BI5" s="11" t="s">
+      <c r="BJ5" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="BJ5" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="BK5" s="11" t="s">
         <v>57</v>
@@ -2054,7 +1945,7 @@
         <v>162</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>87</v>
@@ -2075,62 +1966,62 @@
         <v>84</v>
       </c>
       <c r="K6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q6" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>86</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="W6" s="5" t="s">
         <v>73</v>
       </c>
       <c r="X6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="Y6" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="Z6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AA6" s="5" t="s">
+      <c r="AB6" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="AB6" s="5" t="s">
+      <c r="AC6" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AC6" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="AD6" s="5" t="s">
         <v>71</v>
       </c>
@@ -2153,11 +2044,11 @@
         <v>71</v>
       </c>
       <c r="AK6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AL6" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="AM6" s="5" t="s">
         <v>71</v>
       </c>
@@ -2165,11 +2056,11 @@
         <v>71</v>
       </c>
       <c r="AO6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AP6" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ6" s="5" t="s">
         <v>71</v>
       </c>
@@ -2189,38 +2080,38 @@
         <v>71</v>
       </c>
       <c r="AW6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AX6" s="6" t="s">
-        <v>89</v>
-      </c>
       <c r="AY6" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ6" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA6" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="BC6" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="BD6" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="BE6" s="1" t="s">
-        <v>71</v>
+      <c r="BE6" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="BF6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BG6" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH6" s="1" t="s">
         <v>71</v>
       </c>
@@ -2228,7 +2119,7 @@
         <v>71</v>
       </c>
       <c r="BJ6" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK6" s="1" t="s">
         <v>76</v>
@@ -2240,7 +2131,7 @@
         <v>98</v>
       </c>
       <c r="BN6" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO6" s="1" t="s">
         <v>101</v>
@@ -2269,7 +2160,7 @@
         <v>103</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>87</v>
@@ -2287,62 +2178,62 @@
         <v>84</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q7" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>86</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD7" s="1" t="s">
         <v>71</v>
       </c>
@@ -2365,11 +2256,11 @@
         <v>71</v>
       </c>
       <c r="AK7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AL7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AM7" s="1" t="s">
         <v>71</v>
       </c>
@@ -2377,11 +2268,11 @@
         <v>71</v>
       </c>
       <c r="AO7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ7" s="1" t="s">
         <v>71</v>
       </c>
@@ -2401,38 +2292,38 @@
         <v>71</v>
       </c>
       <c r="AW7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AX7" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY7" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ7" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA7" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC7" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD7" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE7" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BG7" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH7" s="1" t="s">
         <v>71</v>
       </c>
@@ -2440,7 +2331,7 @@
         <v>71</v>
       </c>
       <c r="BJ7" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK7" s="1" t="s">
         <v>76</v>
@@ -2452,7 +2343,7 @@
         <v>98</v>
       </c>
       <c r="BN7" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO7" s="1" t="s">
         <v>101</v>
@@ -2481,7 +2372,7 @@
         <v>106</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>87</v>
@@ -2499,62 +2390,62 @@
         <v>84</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q8" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>86</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y8" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AC8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC8" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD8" s="1" t="s">
         <v>71</v>
       </c>
@@ -2577,11 +2468,11 @@
         <v>71</v>
       </c>
       <c r="AK8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AL8" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AM8" s="1" t="s">
         <v>71</v>
       </c>
@@ -2589,11 +2480,11 @@
         <v>71</v>
       </c>
       <c r="AO8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP8" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ8" s="1" t="s">
         <v>71</v>
       </c>
@@ -2613,38 +2504,38 @@
         <v>71</v>
       </c>
       <c r="AW8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AX8" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY8" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ8" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA8" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC8" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD8" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE8" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BG8" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH8" s="1" t="s">
         <v>71</v>
       </c>
@@ -2652,7 +2543,7 @@
         <v>71</v>
       </c>
       <c r="BJ8" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK8" s="1" t="s">
         <v>76</v>
@@ -2664,7 +2555,7 @@
         <v>98</v>
       </c>
       <c r="BN8" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO8" s="1" t="s">
         <v>101</v>
@@ -2693,7 +2584,7 @@
         <v>109</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>87</v>
@@ -2711,62 +2602,62 @@
         <v>84</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q9" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>86</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD9" s="1" t="s">
         <v>71</v>
       </c>
@@ -2789,11 +2680,11 @@
         <v>71</v>
       </c>
       <c r="AK9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AL9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AM9" s="1" t="s">
         <v>71</v>
       </c>
@@ -2801,11 +2692,11 @@
         <v>71</v>
       </c>
       <c r="AO9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ9" s="1" t="s">
         <v>71</v>
       </c>
@@ -2825,38 +2716,38 @@
         <v>71</v>
       </c>
       <c r="AW9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AX9" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY9" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ9" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA9" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC9" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD9" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE9" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BG9" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH9" s="1" t="s">
         <v>71</v>
       </c>
@@ -2864,7 +2755,7 @@
         <v>71</v>
       </c>
       <c r="BJ9" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK9" s="1" t="s">
         <v>76</v>
@@ -2876,7 +2767,7 @@
         <v>113</v>
       </c>
       <c r="BN9" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO9" s="1" t="s">
         <v>101</v>
@@ -2905,7 +2796,7 @@
         <v>117</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>87</v>
@@ -2923,62 +2814,62 @@
         <v>84</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q10" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>86</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y10" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AB10" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AC10" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC10" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD10" s="1" t="s">
         <v>71</v>
       </c>
@@ -3001,11 +2892,11 @@
         <v>71</v>
       </c>
       <c r="AK10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AL10" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AM10" s="1" t="s">
         <v>71</v>
       </c>
@@ -3013,11 +2904,11 @@
         <v>71</v>
       </c>
       <c r="AO10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP10" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ10" s="1" t="s">
         <v>71</v>
       </c>
@@ -3037,38 +2928,38 @@
         <v>71</v>
       </c>
       <c r="AW10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AX10" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY10" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ10" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA10" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC10" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD10" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE10" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BG10" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH10" s="1" t="s">
         <v>71</v>
       </c>
@@ -3076,7 +2967,7 @@
         <v>71</v>
       </c>
       <c r="BJ10" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK10" s="1" t="s">
         <v>76</v>
@@ -3088,7 +2979,7 @@
         <v>113</v>
       </c>
       <c r="BN10" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO10" s="1" t="s">
         <v>101</v>
@@ -3117,7 +3008,7 @@
         <v>114</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>87</v>
@@ -3135,62 +3026,62 @@
         <v>84</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q11" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>86</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y11" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AC11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC11" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD11" s="1" t="s">
         <v>71</v>
       </c>
@@ -3213,11 +3104,11 @@
         <v>71</v>
       </c>
       <c r="AK11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AL11" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AM11" s="1" t="s">
         <v>71</v>
       </c>
@@ -3225,11 +3116,11 @@
         <v>71</v>
       </c>
       <c r="AO11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP11" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ11" s="1" t="s">
         <v>71</v>
       </c>
@@ -3249,38 +3140,38 @@
         <v>71</v>
       </c>
       <c r="AW11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AX11" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY11" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ11" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA11" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC11" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD11" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE11" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BG11" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH11" s="1" t="s">
         <v>71</v>
       </c>
@@ -3288,7 +3179,7 @@
         <v>71</v>
       </c>
       <c r="BJ11" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK11" s="1" t="s">
         <v>76</v>
@@ -3300,7 +3191,7 @@
         <v>98</v>
       </c>
       <c r="BN11" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO11" s="1" t="s">
         <v>101</v>
@@ -3329,7 +3220,7 @@
         <v>120</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>87</v>
@@ -3347,62 +3238,62 @@
         <v>84</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q12" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>86</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="W12" s="1" t="s">
         <v>73</v>
       </c>
       <c r="X12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="Y12" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AB12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AC12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AC12" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD12" s="1" t="s">
         <v>71</v>
       </c>
@@ -3425,11 +3316,11 @@
         <v>71</v>
       </c>
       <c r="AK12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AL12" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AM12" s="1" t="s">
         <v>71</v>
       </c>
@@ -3437,11 +3328,11 @@
         <v>71</v>
       </c>
       <c r="AO12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AP12" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AQ12" s="1" t="s">
         <v>71</v>
       </c>
@@ -3461,38 +3352,38 @@
         <v>71</v>
       </c>
       <c r="AW12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AX12" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY12" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ12" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA12" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC12" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD12" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE12" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BG12" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH12" s="1" t="s">
         <v>71</v>
       </c>
@@ -3500,7 +3391,7 @@
         <v>71</v>
       </c>
       <c r="BJ12" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK12" s="1" t="s">
         <v>76</v>
@@ -3512,7 +3403,7 @@
         <v>123</v>
       </c>
       <c r="BN12" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO12" s="1" t="s">
         <v>101</v>
@@ -3541,7 +3432,7 @@
         <v>124</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>126</v>
@@ -3559,62 +3450,62 @@
         <v>84</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="M13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q13" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S13" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>125</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="W13" s="1" t="s">
         <v>79</v>
       </c>
       <c r="X13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Y13" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AA13" s="1" t="s">
+      <c r="AB13" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AB13" s="1" t="s">
+      <c r="AC13" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AC13" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD13" s="1" t="s">
         <v>71</v>
       </c>
@@ -3673,38 +3564,38 @@
         <v>71</v>
       </c>
       <c r="AW13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AX13" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY13" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ13" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA13" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BC13" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD13" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE13" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BG13" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH13" s="1" t="s">
         <v>71</v>
       </c>
@@ -3712,7 +3603,7 @@
         <v>71</v>
       </c>
       <c r="BJ13" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK13" s="1" t="s">
         <v>76</v>
@@ -3724,7 +3615,7 @@
         <v>131</v>
       </c>
       <c r="BN13" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO13" s="1" t="s">
         <v>101</v>
@@ -3753,7 +3644,7 @@
         <v>134</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>136</v>
@@ -3771,62 +3662,62 @@
         <v>84</v>
       </c>
       <c r="K14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q14" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S14" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>135</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="W14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="X14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y14" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Y14" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AB14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AC14" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD14" s="1" t="s">
         <v>71</v>
       </c>
@@ -3885,38 +3776,38 @@
         <v>71</v>
       </c>
       <c r="AW14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX14" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AX14" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY14" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ14" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA14" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC14" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD14" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE14" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BG14" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH14" s="1" t="s">
         <v>71</v>
       </c>
@@ -3924,7 +3815,7 @@
         <v>71</v>
       </c>
       <c r="BJ14" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK14" s="1" t="s">
         <v>76</v>
@@ -3936,7 +3827,7 @@
         <v>142</v>
       </c>
       <c r="BN14" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO14" s="1" t="s">
         <v>101</v>
@@ -3962,10 +3853,10 @@
         <v>102</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>136</v>
@@ -3983,62 +3874,62 @@
         <v>84</v>
       </c>
       <c r="K15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="Q15" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="R15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>135</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="W15" s="1" t="s">
         <v>81</v>
       </c>
       <c r="X15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Y15" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="Z15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA15" s="1" t="s">
+      <c r="AB15" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AB15" s="1" t="s">
+      <c r="AC15" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AC15" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="AD15" s="1" t="s">
         <v>71</v>
       </c>
@@ -4097,38 +3988,38 @@
         <v>71</v>
       </c>
       <c r="AW15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AX15" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AX15" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AY15" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AZ15" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="BA15" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="BB15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BC15" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="BD15" s="1" t="s">
         <v>84</v>
       </c>
       <c r="BE15" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="BF15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BG15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BG15" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="BH15" s="1" t="s">
         <v>71</v>
       </c>
@@ -4136,7 +4027,7 @@
         <v>71</v>
       </c>
       <c r="BJ15" s="1" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="BK15" s="1" t="s">
         <v>76</v>
@@ -4148,7 +4039,7 @@
         <v>142</v>
       </c>
       <c r="BN15" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="BO15" s="1" t="s">
         <v>101</v>
@@ -4170,1005 +4061,1005 @@
       </c>
     </row>
     <row r="17" spans="1:72" s="4" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="H17" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>247</v>
-      </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="L17" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="M17" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="M17" s="19" t="s">
+      <c r="N17" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="N17" s="19" t="s">
+      <c r="O17" s="24" t="s">
         <v>227</v>
       </c>
-      <c r="O17" s="19" t="s">
+      <c r="P17" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="P17" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q17" s="19" t="s">
+      <c r="Q17" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="R17" s="24" t="s">
         <v>225</v>
       </c>
-      <c r="R17" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="S17" s="19" t="s">
+      <c r="S17" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="T17" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="T17" s="19" t="s">
+      <c r="U17" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="U17" s="19" t="s">
+      <c r="V17" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="V17" s="19" t="s">
+      <c r="W17" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="W17" s="19" t="s">
+      <c r="X17" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="X17" s="19" t="s">
+      <c r="Y17" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="Y17" s="19" t="s">
+      <c r="Z17" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="Z17" s="19" t="s">
+      <c r="AA17" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="AA17" s="19" t="s">
+      <c r="AB17" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="AB17" s="19" t="s">
+      <c r="AC17" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="AC17" s="19" t="s">
+      <c r="AD17" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="AD17" s="19" t="s">
+      <c r="AE17" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="AE17" s="19" t="s">
+      <c r="AF17" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="AF17" s="19" t="s">
+      <c r="AG17" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="AG17" s="18" t="s">
+      <c r="AH17" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="AH17" s="18" t="s">
+      <c r="AI17" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="AI17" s="18" t="s">
+      <c r="AJ17" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="AJ17" s="18" t="s">
+      <c r="AK17" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="AK17" s="19" t="s">
+      <c r="AL17" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="AL17" s="18" t="s">
+      <c r="AM17" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="AM17" s="18" t="s">
+      <c r="AN17" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="AN17" s="18" t="s">
+      <c r="AO17" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="AO17" s="19" t="s">
+      <c r="AP17" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="AP17" s="18" t="s">
+      <c r="AQ17" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="AQ17" s="18" t="s">
+      <c r="AR17" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="AR17" s="18" t="s">
+      <c r="AS17" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="AS17" s="19" t="s">
+      <c r="AT17" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="AT17" s="18" t="s">
+      <c r="AU17" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="AU17" s="18" t="s">
+      <c r="AV17" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="AV17" s="18" t="s">
+      <c r="AW17" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="AW17" s="18" t="s">
+      <c r="AX17" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="AX17" s="23" t="s">
+      <c r="AY17" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="AY17" s="23" t="s">
+      <c r="AZ17" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="AZ17" s="23" t="s">
-        <v>270</v>
-      </c>
       <c r="BA17" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB17" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="BB17" s="23" t="s">
+      <c r="BC17" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="BC17" s="23" t="s">
+      <c r="BD17" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="BD17" s="23" t="s">
+      <c r="BE17" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="BE17" s="17" t="s">
+      <c r="BF17" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="BF17" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="BG17" s="15" t="s">
+      <c r="BG17" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="BH17" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="BI17" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="BH17" s="15" t="s">
+      <c r="BJ17" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="BI17" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="BJ17" s="38" t="s">
+      <c r="BK17" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="BL17" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="BM17" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="BN17" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="BO17" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="BP17" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="BK17" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="BL17" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="BM17" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="BN17" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="BO17" s="24" t="s">
+      <c r="BQ17" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="BR17" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="BS17" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="BP17" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="BQ17" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="BR17" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="BS17" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="BT17" s="20" t="s">
+      <c r="BT17" s="28" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:72">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
-      <c r="W18" s="19"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="19"/>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="19"/>
-      <c r="AC18" s="19"/>
-      <c r="AD18" s="19"/>
-      <c r="AE18" s="19"/>
-      <c r="AF18" s="19"/>
-      <c r="AG18" s="18"/>
-      <c r="AH18" s="18"/>
-      <c r="AI18" s="18"/>
-      <c r="AJ18" s="18"/>
-      <c r="AK18" s="19"/>
-      <c r="AL18" s="18"/>
-      <c r="AM18" s="18"/>
-      <c r="AN18" s="18"/>
-      <c r="AO18" s="19"/>
-      <c r="AP18" s="18"/>
-      <c r="AQ18" s="18"/>
-      <c r="AR18" s="18"/>
-      <c r="AS18" s="19"/>
-      <c r="AT18" s="18"/>
-      <c r="AU18" s="18"/>
-      <c r="AV18" s="18"/>
-      <c r="AW18" s="18"/>
-      <c r="AX18" s="23"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
+      <c r="T18" s="24"/>
+      <c r="U18" s="24"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+      <c r="Y18" s="24"/>
+      <c r="Z18" s="24"/>
+      <c r="AA18" s="24"/>
+      <c r="AB18" s="24"/>
+      <c r="AC18" s="24"/>
+      <c r="AD18" s="24"/>
+      <c r="AE18" s="24"/>
+      <c r="AF18" s="24"/>
+      <c r="AG18" s="24"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="24"/>
+      <c r="AM18" s="14"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="14"/>
+      <c r="AP18" s="24"/>
+      <c r="AQ18" s="14"/>
+      <c r="AR18" s="14"/>
+      <c r="AS18" s="14"/>
+      <c r="AT18" s="24"/>
+      <c r="AU18" s="14"/>
+      <c r="AV18" s="14"/>
+      <c r="AW18" s="14"/>
+      <c r="AX18" s="14"/>
       <c r="AY18" s="23"/>
       <c r="AZ18" s="23"/>
       <c r="BA18" s="23"/>
       <c r="BB18" s="23"/>
       <c r="BC18" s="23"/>
       <c r="BD18" s="23"/>
-      <c r="BE18" s="17"/>
-      <c r="BF18" s="15"/>
-      <c r="BG18" s="15"/>
-      <c r="BH18" s="15"/>
-      <c r="BI18" s="15"/>
-      <c r="BJ18" s="38"/>
-      <c r="BK18" s="24"/>
-      <c r="BL18" s="24"/>
-      <c r="BM18" s="24"/>
-      <c r="BN18" s="24"/>
-      <c r="BO18" s="24"/>
-      <c r="BP18" s="24"/>
-      <c r="BQ18" s="24"/>
-      <c r="BR18" s="24"/>
-      <c r="BS18" s="24"/>
-      <c r="BT18" s="20"/>
+      <c r="BE18" s="23"/>
+      <c r="BF18" s="29"/>
+      <c r="BG18" s="19"/>
+      <c r="BH18" s="19"/>
+      <c r="BI18" s="19"/>
+      <c r="BJ18" s="19"/>
+      <c r="BK18" s="16"/>
+      <c r="BL18" s="16"/>
+      <c r="BM18" s="16"/>
+      <c r="BN18" s="16"/>
+      <c r="BO18" s="16"/>
+      <c r="BP18" s="16"/>
+      <c r="BQ18" s="16"/>
+      <c r="BR18" s="16"/>
+      <c r="BS18" s="16"/>
+      <c r="BT18" s="28"/>
     </row>
     <row r="19" spans="1:72">
-      <c r="A19" s="21"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="19"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="19"/>
-      <c r="AA19" s="19"/>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
-      <c r="AD19" s="19"/>
-      <c r="AE19" s="19"/>
-      <c r="AF19" s="19"/>
-      <c r="AG19" s="18"/>
-      <c r="AH19" s="18"/>
-      <c r="AI19" s="18"/>
-      <c r="AJ19" s="18"/>
-      <c r="AK19" s="19"/>
-      <c r="AL19" s="18"/>
-      <c r="AM19" s="18"/>
-      <c r="AN19" s="18"/>
-      <c r="AO19" s="19"/>
-      <c r="AP19" s="18"/>
-      <c r="AQ19" s="18"/>
-      <c r="AR19" s="18"/>
-      <c r="AS19" s="19"/>
-      <c r="AT19" s="18"/>
-      <c r="AU19" s="18"/>
-      <c r="AV19" s="18"/>
-      <c r="AW19" s="18"/>
-      <c r="AX19" s="23"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="24"/>
+      <c r="AB19" s="24"/>
+      <c r="AC19" s="24"/>
+      <c r="AD19" s="24"/>
+      <c r="AE19" s="24"/>
+      <c r="AF19" s="24"/>
+      <c r="AG19" s="24"/>
+      <c r="AH19" s="14"/>
+      <c r="AI19" s="14"/>
+      <c r="AJ19" s="14"/>
+      <c r="AK19" s="14"/>
+      <c r="AL19" s="24"/>
+      <c r="AM19" s="14"/>
+      <c r="AN19" s="14"/>
+      <c r="AO19" s="14"/>
+      <c r="AP19" s="24"/>
+      <c r="AQ19" s="14"/>
+      <c r="AR19" s="14"/>
+      <c r="AS19" s="14"/>
+      <c r="AT19" s="24"/>
+      <c r="AU19" s="14"/>
+      <c r="AV19" s="14"/>
+      <c r="AW19" s="14"/>
+      <c r="AX19" s="14"/>
       <c r="AY19" s="23"/>
       <c r="AZ19" s="23"/>
       <c r="BA19" s="23"/>
       <c r="BB19" s="23"/>
       <c r="BC19" s="23"/>
       <c r="BD19" s="23"/>
-      <c r="BE19" s="17"/>
-      <c r="BF19" s="15"/>
-      <c r="BG19" s="15"/>
-      <c r="BH19" s="15"/>
-      <c r="BI19" s="15"/>
-      <c r="BJ19" s="38"/>
-      <c r="BK19" s="24"/>
-      <c r="BL19" s="24"/>
-      <c r="BM19" s="24"/>
-      <c r="BN19" s="24"/>
-      <c r="BO19" s="24"/>
-      <c r="BP19" s="24"/>
-      <c r="BQ19" s="24"/>
-      <c r="BR19" s="24"/>
-      <c r="BS19" s="24"/>
-      <c r="BT19" s="20"/>
+      <c r="BE19" s="23"/>
+      <c r="BF19" s="29"/>
+      <c r="BG19" s="19"/>
+      <c r="BH19" s="19"/>
+      <c r="BI19" s="19"/>
+      <c r="BJ19" s="19"/>
+      <c r="BK19" s="16"/>
+      <c r="BL19" s="16"/>
+      <c r="BM19" s="16"/>
+      <c r="BN19" s="16"/>
+      <c r="BO19" s="16"/>
+      <c r="BP19" s="16"/>
+      <c r="BQ19" s="16"/>
+      <c r="BR19" s="16"/>
+      <c r="BS19" s="16"/>
+      <c r="BT19" s="28"/>
     </row>
     <row r="20" spans="1:72">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="19"/>
-      <c r="W20" s="19"/>
-      <c r="X20" s="19"/>
-      <c r="Y20" s="19"/>
-      <c r="Z20" s="19"/>
-      <c r="AA20" s="19"/>
-      <c r="AB20" s="19"/>
-      <c r="AC20" s="19"/>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="19"/>
-      <c r="AF20" s="19"/>
-      <c r="AG20" s="18"/>
-      <c r="AH20" s="18"/>
-      <c r="AI20" s="18"/>
-      <c r="AJ20" s="18"/>
-      <c r="AK20" s="19"/>
-      <c r="AL20" s="18"/>
-      <c r="AM20" s="18"/>
-      <c r="AN20" s="18"/>
-      <c r="AO20" s="19"/>
-      <c r="AP20" s="18"/>
-      <c r="AQ20" s="18"/>
-      <c r="AR20" s="18"/>
-      <c r="AS20" s="19"/>
-      <c r="AT20" s="18"/>
-      <c r="AU20" s="18"/>
-      <c r="AV20" s="18"/>
-      <c r="AW20" s="18"/>
-      <c r="AX20" s="23"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+      <c r="T20" s="24"/>
+      <c r="U20" s="24"/>
+      <c r="V20" s="24"/>
+      <c r="W20" s="24"/>
+      <c r="X20" s="24"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
+      <c r="AD20" s="24"/>
+      <c r="AE20" s="24"/>
+      <c r="AF20" s="24"/>
+      <c r="AG20" s="24"/>
+      <c r="AH20" s="14"/>
+      <c r="AI20" s="14"/>
+      <c r="AJ20" s="14"/>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="24"/>
+      <c r="AM20" s="14"/>
+      <c r="AN20" s="14"/>
+      <c r="AO20" s="14"/>
+      <c r="AP20" s="24"/>
+      <c r="AQ20" s="14"/>
+      <c r="AR20" s="14"/>
+      <c r="AS20" s="14"/>
+      <c r="AT20" s="24"/>
+      <c r="AU20" s="14"/>
+      <c r="AV20" s="14"/>
+      <c r="AW20" s="14"/>
+      <c r="AX20" s="14"/>
       <c r="AY20" s="23"/>
       <c r="AZ20" s="23"/>
       <c r="BA20" s="23"/>
       <c r="BB20" s="23"/>
       <c r="BC20" s="23"/>
       <c r="BD20" s="23"/>
-      <c r="BE20" s="17"/>
-      <c r="BF20" s="15"/>
-      <c r="BG20" s="15"/>
-      <c r="BH20" s="15"/>
-      <c r="BI20" s="15"/>
-      <c r="BJ20" s="38"/>
-      <c r="BK20" s="24"/>
-      <c r="BL20" s="24"/>
-      <c r="BM20" s="24"/>
-      <c r="BN20" s="24"/>
-      <c r="BO20" s="24"/>
-      <c r="BP20" s="24"/>
-      <c r="BQ20" s="24"/>
-      <c r="BR20" s="24"/>
-      <c r="BS20" s="24"/>
-      <c r="BT20" s="20"/>
+      <c r="BE20" s="23"/>
+      <c r="BF20" s="29"/>
+      <c r="BG20" s="19"/>
+      <c r="BH20" s="19"/>
+      <c r="BI20" s="19"/>
+      <c r="BJ20" s="19"/>
+      <c r="BK20" s="16"/>
+      <c r="BL20" s="16"/>
+      <c r="BM20" s="16"/>
+      <c r="BN20" s="16"/>
+      <c r="BO20" s="16"/>
+      <c r="BP20" s="16"/>
+      <c r="BQ20" s="16"/>
+      <c r="BR20" s="16"/>
+      <c r="BS20" s="16"/>
+      <c r="BT20" s="28"/>
     </row>
     <row r="21" spans="1:72">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="19"/>
-      <c r="AF21" s="19"/>
-      <c r="AG21" s="18"/>
-      <c r="AH21" s="18"/>
-      <c r="AI21" s="18"/>
-      <c r="AJ21" s="18"/>
-      <c r="AK21" s="19"/>
-      <c r="AL21" s="18"/>
-      <c r="AM21" s="18"/>
-      <c r="AN21" s="18"/>
-      <c r="AO21" s="19"/>
-      <c r="AP21" s="18"/>
-      <c r="AQ21" s="18"/>
-      <c r="AR21" s="18"/>
-      <c r="AS21" s="19"/>
-      <c r="AT21" s="18"/>
-      <c r="AU21" s="18"/>
-      <c r="AV21" s="18"/>
-      <c r="AW21" s="18"/>
-      <c r="AX21" s="23"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="24"/>
+      <c r="AD21" s="24"/>
+      <c r="AE21" s="24"/>
+      <c r="AF21" s="24"/>
+      <c r="AG21" s="24"/>
+      <c r="AH21" s="14"/>
+      <c r="AI21" s="14"/>
+      <c r="AJ21" s="14"/>
+      <c r="AK21" s="14"/>
+      <c r="AL21" s="24"/>
+      <c r="AM21" s="14"/>
+      <c r="AN21" s="14"/>
+      <c r="AO21" s="14"/>
+      <c r="AP21" s="24"/>
+      <c r="AQ21" s="14"/>
+      <c r="AR21" s="14"/>
+      <c r="AS21" s="14"/>
+      <c r="AT21" s="24"/>
+      <c r="AU21" s="14"/>
+      <c r="AV21" s="14"/>
+      <c r="AW21" s="14"/>
+      <c r="AX21" s="14"/>
       <c r="AY21" s="23"/>
       <c r="AZ21" s="23"/>
       <c r="BA21" s="23"/>
       <c r="BB21" s="23"/>
       <c r="BC21" s="23"/>
       <c r="BD21" s="23"/>
-      <c r="BE21" s="17"/>
-      <c r="BF21" s="15"/>
-      <c r="BG21" s="15"/>
-      <c r="BH21" s="15"/>
-      <c r="BI21" s="15"/>
-      <c r="BJ21" s="38"/>
-      <c r="BK21" s="24"/>
-      <c r="BL21" s="24"/>
-      <c r="BM21" s="24"/>
-      <c r="BN21" s="24"/>
-      <c r="BO21" s="24"/>
-      <c r="BP21" s="24"/>
-      <c r="BQ21" s="24"/>
-      <c r="BR21" s="24"/>
-      <c r="BS21" s="24"/>
-      <c r="BT21" s="20"/>
+      <c r="BE21" s="23"/>
+      <c r="BF21" s="29"/>
+      <c r="BG21" s="19"/>
+      <c r="BH21" s="19"/>
+      <c r="BI21" s="19"/>
+      <c r="BJ21" s="19"/>
+      <c r="BK21" s="16"/>
+      <c r="BL21" s="16"/>
+      <c r="BM21" s="16"/>
+      <c r="BN21" s="16"/>
+      <c r="BO21" s="16"/>
+      <c r="BP21" s="16"/>
+      <c r="BQ21" s="16"/>
+      <c r="BR21" s="16"/>
+      <c r="BS21" s="16"/>
+      <c r="BT21" s="28"/>
     </row>
     <row r="22" spans="1:72">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="19"/>
-      <c r="Y22" s="19"/>
-      <c r="Z22" s="19"/>
-      <c r="AA22" s="19"/>
-      <c r="AB22" s="19"/>
-      <c r="AC22" s="19"/>
-      <c r="AD22" s="19"/>
-      <c r="AE22" s="19"/>
-      <c r="AF22" s="19"/>
-      <c r="AG22" s="18"/>
-      <c r="AH22" s="18"/>
-      <c r="AI22" s="18"/>
-      <c r="AJ22" s="18"/>
-      <c r="AK22" s="19"/>
-      <c r="AL22" s="18"/>
-      <c r="AM22" s="18"/>
-      <c r="AN22" s="18"/>
-      <c r="AO22" s="19"/>
-      <c r="AP22" s="18"/>
-      <c r="AQ22" s="18"/>
-      <c r="AR22" s="18"/>
-      <c r="AS22" s="19"/>
-      <c r="AT22" s="18"/>
-      <c r="AU22" s="18"/>
-      <c r="AV22" s="18"/>
-      <c r="AW22" s="18"/>
-      <c r="AX22" s="23"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
+      <c r="T22" s="24"/>
+      <c r="U22" s="24"/>
+      <c r="V22" s="24"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="24"/>
+      <c r="Y22" s="24"/>
+      <c r="Z22" s="24"/>
+      <c r="AA22" s="24"/>
+      <c r="AB22" s="24"/>
+      <c r="AC22" s="24"/>
+      <c r="AD22" s="24"/>
+      <c r="AE22" s="24"/>
+      <c r="AF22" s="24"/>
+      <c r="AG22" s="24"/>
+      <c r="AH22" s="14"/>
+      <c r="AI22" s="14"/>
+      <c r="AJ22" s="14"/>
+      <c r="AK22" s="14"/>
+      <c r="AL22" s="24"/>
+      <c r="AM22" s="14"/>
+      <c r="AN22" s="14"/>
+      <c r="AO22" s="14"/>
+      <c r="AP22" s="24"/>
+      <c r="AQ22" s="14"/>
+      <c r="AR22" s="14"/>
+      <c r="AS22" s="14"/>
+      <c r="AT22" s="24"/>
+      <c r="AU22" s="14"/>
+      <c r="AV22" s="14"/>
+      <c r="AW22" s="14"/>
+      <c r="AX22" s="14"/>
       <c r="AY22" s="23"/>
       <c r="AZ22" s="23"/>
       <c r="BA22" s="23"/>
       <c r="BB22" s="23"/>
       <c r="BC22" s="23"/>
       <c r="BD22" s="23"/>
-      <c r="BE22" s="17"/>
-      <c r="BF22" s="15"/>
-      <c r="BG22" s="15"/>
-      <c r="BH22" s="15"/>
-      <c r="BI22" s="15"/>
-      <c r="BJ22" s="38"/>
-      <c r="BK22" s="24"/>
-      <c r="BL22" s="24"/>
-      <c r="BM22" s="24"/>
-      <c r="BN22" s="24"/>
-      <c r="BO22" s="24"/>
-      <c r="BP22" s="24"/>
-      <c r="BQ22" s="24"/>
-      <c r="BR22" s="24"/>
-      <c r="BS22" s="24"/>
-      <c r="BT22" s="20"/>
+      <c r="BE22" s="23"/>
+      <c r="BF22" s="29"/>
+      <c r="BG22" s="19"/>
+      <c r="BH22" s="19"/>
+      <c r="BI22" s="19"/>
+      <c r="BJ22" s="19"/>
+      <c r="BK22" s="16"/>
+      <c r="BL22" s="16"/>
+      <c r="BM22" s="16"/>
+      <c r="BN22" s="16"/>
+      <c r="BO22" s="16"/>
+      <c r="BP22" s="16"/>
+      <c r="BQ22" s="16"/>
+      <c r="BR22" s="16"/>
+      <c r="BS22" s="16"/>
+      <c r="BT22" s="28"/>
     </row>
     <row r="23" spans="1:72">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="18"/>
-      <c r="AH23" s="18"/>
-      <c r="AI23" s="18"/>
-      <c r="AJ23" s="18"/>
-      <c r="AK23" s="19"/>
-      <c r="AL23" s="18"/>
-      <c r="AM23" s="18"/>
-      <c r="AN23" s="18"/>
-      <c r="AO23" s="19"/>
-      <c r="AP23" s="18"/>
-      <c r="AQ23" s="18"/>
-      <c r="AR23" s="18"/>
-      <c r="AS23" s="19"/>
-      <c r="AT23" s="18"/>
-      <c r="AU23" s="18"/>
-      <c r="AV23" s="18"/>
-      <c r="AW23" s="18"/>
-      <c r="AX23" s="23"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="24"/>
+      <c r="V23" s="24"/>
+      <c r="W23" s="24"/>
+      <c r="X23" s="24"/>
+      <c r="Y23" s="24"/>
+      <c r="Z23" s="24"/>
+      <c r="AA23" s="24"/>
+      <c r="AB23" s="24"/>
+      <c r="AC23" s="24"/>
+      <c r="AD23" s="24"/>
+      <c r="AE23" s="24"/>
+      <c r="AF23" s="24"/>
+      <c r="AG23" s="24"/>
+      <c r="AH23" s="14"/>
+      <c r="AI23" s="14"/>
+      <c r="AJ23" s="14"/>
+      <c r="AK23" s="14"/>
+      <c r="AL23" s="24"/>
+      <c r="AM23" s="14"/>
+      <c r="AN23" s="14"/>
+      <c r="AO23" s="14"/>
+      <c r="AP23" s="24"/>
+      <c r="AQ23" s="14"/>
+      <c r="AR23" s="14"/>
+      <c r="AS23" s="14"/>
+      <c r="AT23" s="24"/>
+      <c r="AU23" s="14"/>
+      <c r="AV23" s="14"/>
+      <c r="AW23" s="14"/>
+      <c r="AX23" s="14"/>
       <c r="AY23" s="23"/>
       <c r="AZ23" s="23"/>
       <c r="BA23" s="23"/>
       <c r="BB23" s="23"/>
       <c r="BC23" s="23"/>
       <c r="BD23" s="23"/>
-      <c r="BE23" s="17"/>
-      <c r="BF23" s="15"/>
-      <c r="BG23" s="15"/>
-      <c r="BH23" s="15"/>
-      <c r="BI23" s="15"/>
-      <c r="BJ23" s="38"/>
-      <c r="BK23" s="24"/>
-      <c r="BL23" s="24"/>
-      <c r="BM23" s="24"/>
-      <c r="BN23" s="24"/>
-      <c r="BO23" s="24"/>
-      <c r="BP23" s="24"/>
-      <c r="BQ23" s="24"/>
-      <c r="BR23" s="24"/>
-      <c r="BS23" s="24"/>
-      <c r="BT23" s="20"/>
+      <c r="BE23" s="23"/>
+      <c r="BF23" s="29"/>
+      <c r="BG23" s="19"/>
+      <c r="BH23" s="19"/>
+      <c r="BI23" s="19"/>
+      <c r="BJ23" s="19"/>
+      <c r="BK23" s="16"/>
+      <c r="BL23" s="16"/>
+      <c r="BM23" s="16"/>
+      <c r="BN23" s="16"/>
+      <c r="BO23" s="16"/>
+      <c r="BP23" s="16"/>
+      <c r="BQ23" s="16"/>
+      <c r="BR23" s="16"/>
+      <c r="BS23" s="16"/>
+      <c r="BT23" s="28"/>
     </row>
     <row r="24" spans="1:72">
-      <c r="BF24" s="15" t="s">
-        <v>251</v>
+      <c r="BG24" s="19" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:72" ht="11.25" customHeight="1">
       <c r="F25" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="M25" s="18" t="s">
+      <c r="N25" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="O25" s="18" t="s">
+      <c r="P25" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="Q25" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="R25" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="AH25" s="19" t="s">
+      <c r="R25" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="S25" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="AI25" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="AI25" s="18" t="s">
+      <c r="AJ25" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="AL25" s="19" t="s">
+      <c r="AM25" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="AM25" s="18" t="s">
+      <c r="AN25" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="AP25" s="19" t="s">
+      <c r="AQ25" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="AQ25" s="18" t="s">
+      <c r="AR25" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="AT25" s="19" t="s">
+      <c r="AU25" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="AU25" s="18" t="s">
+      <c r="AV25" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="AW25" s="18" t="s">
+      <c r="AX25" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="AY25" s="1" t="s">
+      <c r="AZ25" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BD25" s="1" t="s">
+      <c r="BE25" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BE25" s="17" t="s">
+      <c r="BF25" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="BF25" s="15"/>
+      <c r="BG25" s="19"/>
     </row>
     <row r="26" spans="1:72">
       <c r="F26" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="M26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="AH26" s="19"/>
-      <c r="AI26" s="18"/>
-      <c r="AL26" s="19"/>
-      <c r="AM26" s="18"/>
-      <c r="AP26" s="19"/>
-      <c r="AQ26" s="18"/>
-      <c r="AT26" s="19"/>
-      <c r="AU26" s="18"/>
-      <c r="AW26" s="18"/>
-      <c r="AY26" s="1" t="s">
+      <c r="N26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="AI26" s="24"/>
+      <c r="AJ26" s="14"/>
+      <c r="AM26" s="24"/>
+      <c r="AN26" s="14"/>
+      <c r="AQ26" s="24"/>
+      <c r="AR26" s="14"/>
+      <c r="AU26" s="24"/>
+      <c r="AV26" s="14"/>
+      <c r="AX26" s="14"/>
+      <c r="AZ26" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="BD26" s="3" t="s">
+      <c r="BE26" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="BE26" s="17"/>
-      <c r="BF26" s="15"/>
+      <c r="BF26" s="29"/>
+      <c r="BG26" s="19"/>
     </row>
     <row r="27" spans="1:72">
       <c r="F27" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="AH27" s="19"/>
-      <c r="AI27" s="18"/>
-      <c r="AL27" s="19"/>
-      <c r="AM27" s="18"/>
-      <c r="AP27" s="19"/>
-      <c r="AQ27" s="18"/>
-      <c r="AT27" s="19"/>
-      <c r="AU27" s="18"/>
-      <c r="AW27" s="18"/>
-      <c r="AY27" s="1" t="s">
+      <c r="N27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="AI27" s="24"/>
+      <c r="AJ27" s="14"/>
+      <c r="AM27" s="24"/>
+      <c r="AN27" s="14"/>
+      <c r="AQ27" s="24"/>
+      <c r="AR27" s="14"/>
+      <c r="AU27" s="24"/>
+      <c r="AV27" s="14"/>
+      <c r="AX27" s="14"/>
+      <c r="AZ27" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="BD27" s="3" t="s">
+      <c r="BE27" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="BE27" s="17"/>
-      <c r="BF27" s="15"/>
+      <c r="BF27" s="29"/>
+      <c r="BG27" s="19"/>
     </row>
     <row r="28" spans="1:72">
       <c r="F28" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="AH28" s="19"/>
-      <c r="AI28" s="18"/>
-      <c r="AL28" s="19"/>
-      <c r="AM28" s="18"/>
-      <c r="AP28" s="19"/>
-      <c r="AQ28" s="18"/>
-      <c r="AT28" s="19"/>
-      <c r="AU28" s="18"/>
-      <c r="AW28" s="18"/>
-      <c r="BD28" s="3" t="s">
+      <c r="N28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="AI28" s="24"/>
+      <c r="AJ28" s="14"/>
+      <c r="AM28" s="24"/>
+      <c r="AN28" s="14"/>
+      <c r="AQ28" s="24"/>
+      <c r="AR28" s="14"/>
+      <c r="AU28" s="24"/>
+      <c r="AV28" s="14"/>
+      <c r="AX28" s="14"/>
+      <c r="BE28" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="BE28" s="17"/>
-      <c r="BF28" s="15"/>
+      <c r="BF28" s="29"/>
+      <c r="BG28" s="19"/>
     </row>
     <row r="29" spans="1:72">
       <c r="F29" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="AH29" s="19"/>
-      <c r="AI29" s="18"/>
-      <c r="AL29" s="19"/>
-      <c r="AM29" s="18"/>
-      <c r="AP29" s="19"/>
-      <c r="AQ29" s="18"/>
-      <c r="AT29" s="19"/>
-      <c r="AU29" s="18"/>
-      <c r="AW29" s="18"/>
-      <c r="BD29" s="3" t="s">
+      <c r="N29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="AI29" s="24"/>
+      <c r="AJ29" s="14"/>
+      <c r="AM29" s="24"/>
+      <c r="AN29" s="14"/>
+      <c r="AQ29" s="24"/>
+      <c r="AR29" s="14"/>
+      <c r="AU29" s="24"/>
+      <c r="AV29" s="14"/>
+      <c r="AX29" s="14"/>
+      <c r="BE29" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="BE29" s="17"/>
-      <c r="BF29" s="15"/>
+      <c r="BF29" s="29"/>
+      <c r="BG29" s="19"/>
     </row>
     <row r="30" spans="1:72">
       <c r="F30" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="M30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="AH30" s="19"/>
-      <c r="AI30" s="18"/>
-      <c r="AL30" s="19"/>
-      <c r="AM30" s="18"/>
-      <c r="AP30" s="19"/>
-      <c r="AQ30" s="18"/>
-      <c r="AT30" s="19"/>
-      <c r="AU30" s="18"/>
-      <c r="AW30" s="18"/>
-      <c r="BD30" s="3" t="s">
+      <c r="N30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="AI30" s="24"/>
+      <c r="AJ30" s="14"/>
+      <c r="AM30" s="24"/>
+      <c r="AN30" s="14"/>
+      <c r="AQ30" s="24"/>
+      <c r="AR30" s="14"/>
+      <c r="AU30" s="24"/>
+      <c r="AV30" s="14"/>
+      <c r="AX30" s="14"/>
+      <c r="BE30" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="BE30" s="17"/>
-      <c r="BF30" s="15"/>
+      <c r="BF30" s="29"/>
+      <c r="BG30" s="19"/>
     </row>
     <row r="31" spans="1:72">
-      <c r="M31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="AW31" s="18"/>
-      <c r="BD31" s="3" t="s">
+      <c r="N31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="AX31" s="14"/>
+      <c r="BE31" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="BE31" s="17"/>
+      <c r="BF31" s="29"/>
     </row>
     <row r="32" spans="1:72">
-      <c r="BD32" s="3" t="s">
+      <c r="BE32" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="BE32" s="3"/>
-    </row>
-    <row r="33" spans="18:57" ht="11.25" customHeight="1">
-      <c r="R33" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="BD33" s="3" t="s">
+      <c r="BF32" s="3"/>
+    </row>
+    <row r="33" spans="19:58" ht="11.25" customHeight="1">
+      <c r="S33" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="BE33" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="BE33" s="16" t="s">
+      <c r="BF33" s="31" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="18:57">
-      <c r="R34" s="18"/>
-      <c r="BD34" s="3" t="s">
+    <row r="34" spans="19:58">
+      <c r="S34" s="14"/>
+      <c r="BE34" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="BE34" s="16"/>
-    </row>
-    <row r="35" spans="18:57">
-      <c r="R35" s="18"/>
-      <c r="BD35" s="3" t="s">
+      <c r="BF34" s="31"/>
+    </row>
+    <row r="35" spans="19:58">
+      <c r="S35" s="14"/>
+      <c r="BE35" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="BE35" s="16"/>
-    </row>
-    <row r="36" spans="18:57">
-      <c r="R36" s="18"/>
-      <c r="BD36" s="3" t="s">
+      <c r="BF35" s="31"/>
+    </row>
+    <row r="36" spans="19:58">
+      <c r="S36" s="14"/>
+      <c r="BE36" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="BE36" s="16"/>
-    </row>
-    <row r="37" spans="18:57">
-      <c r="R37" s="18"/>
-      <c r="BD37" s="3" t="s">
+      <c r="BF36" s="31"/>
+    </row>
+    <row r="37" spans="19:58">
+      <c r="S37" s="14"/>
+      <c r="BE37" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="BE37" s="3"/>
-    </row>
-    <row r="38" spans="18:57">
-      <c r="BE38" s="3"/>
-    </row>
-    <row r="39" spans="18:57" ht="11.25" customHeight="1"/>
+      <c r="BF37" s="3"/>
+    </row>
+    <row r="38" spans="19:58">
+      <c r="BF38" s="3"/>
+    </row>
+    <row r="39" spans="19:58" ht="11.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="AX2:BD4"/>
-    <mergeCell ref="R33:R37"/>
-    <mergeCell ref="BF2:BI4"/>
-    <mergeCell ref="BP17:BP23"/>
-    <mergeCell ref="BQ17:BQ23"/>
-    <mergeCell ref="BR17:BR23"/>
-    <mergeCell ref="BJ2:BT4"/>
-    <mergeCell ref="I2:AW4"/>
-    <mergeCell ref="Q25:Q31"/>
-    <mergeCell ref="R25:R31"/>
-    <mergeCell ref="BN17:BN23"/>
-    <mergeCell ref="BO17:BO23"/>
-    <mergeCell ref="O25:O31"/>
-    <mergeCell ref="BJ17:BJ23"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="BG24:BG30"/>
+    <mergeCell ref="BF33:BF36"/>
+    <mergeCell ref="BF25:BF31"/>
+    <mergeCell ref="AX17:AX23"/>
+    <mergeCell ref="AX25:AX31"/>
+    <mergeCell ref="N17:N23"/>
+    <mergeCell ref="N25:N31"/>
+    <mergeCell ref="AR25:AR30"/>
+    <mergeCell ref="AU25:AU30"/>
+    <mergeCell ref="AV25:AV30"/>
+    <mergeCell ref="AM25:AM30"/>
+    <mergeCell ref="AN25:AN30"/>
+    <mergeCell ref="AQ25:AQ30"/>
+    <mergeCell ref="AI17:AI23"/>
+    <mergeCell ref="AI25:AI30"/>
+    <mergeCell ref="BT17:BT23"/>
+    <mergeCell ref="AE17:AE23"/>
+    <mergeCell ref="AF17:AF23"/>
+    <mergeCell ref="AH17:AH23"/>
     <mergeCell ref="BF17:BF23"/>
-    <mergeCell ref="BG17:BG23"/>
-    <mergeCell ref="BH17:BH23"/>
+    <mergeCell ref="AS17:AS23"/>
+    <mergeCell ref="AT17:AT23"/>
+    <mergeCell ref="AU17:AU23"/>
+    <mergeCell ref="AV17:AV23"/>
+    <mergeCell ref="AN17:AN23"/>
+    <mergeCell ref="AO17:AO23"/>
+    <mergeCell ref="AP17:AP23"/>
+    <mergeCell ref="AQ17:AQ23"/>
+    <mergeCell ref="AK17:AK23"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="AB17:AB23"/>
+    <mergeCell ref="AC17:AC23"/>
+    <mergeCell ref="W17:W23"/>
+    <mergeCell ref="X17:X23"/>
+    <mergeCell ref="L17:L23"/>
+    <mergeCell ref="M17:M23"/>
+    <mergeCell ref="J17:J23"/>
+    <mergeCell ref="T17:T23"/>
+    <mergeCell ref="U17:U23"/>
+    <mergeCell ref="D17:D23"/>
+    <mergeCell ref="R17:R23"/>
+    <mergeCell ref="BL17:BL23"/>
+    <mergeCell ref="BM17:BM23"/>
+    <mergeCell ref="BA17:BA23"/>
+    <mergeCell ref="AY17:AY23"/>
+    <mergeCell ref="AZ17:AZ23"/>
+    <mergeCell ref="V17:V23"/>
+    <mergeCell ref="BB17:BB23"/>
+    <mergeCell ref="AM17:AM23"/>
+    <mergeCell ref="AR17:AR23"/>
+    <mergeCell ref="AW17:AW23"/>
+    <mergeCell ref="AL17:AL23"/>
+    <mergeCell ref="Y17:Y23"/>
+    <mergeCell ref="BC17:BC23"/>
+    <mergeCell ref="AA17:AA23"/>
+    <mergeCell ref="AG17:AG23"/>
     <mergeCell ref="B2:G4"/>
-    <mergeCell ref="BE2:BE4"/>
-    <mergeCell ref="BC17:BC23"/>
+    <mergeCell ref="BF2:BF4"/>
     <mergeCell ref="BD17:BD23"/>
-    <mergeCell ref="Y17:Y23"/>
-    <mergeCell ref="AC17:AC23"/>
+    <mergeCell ref="BE17:BE23"/>
+    <mergeCell ref="Z17:Z23"/>
+    <mergeCell ref="AD17:AD23"/>
     <mergeCell ref="B17:B23"/>
     <mergeCell ref="E17:E23"/>
     <mergeCell ref="F17:F23"/>
     <mergeCell ref="G17:G23"/>
     <mergeCell ref="H17:H23"/>
     <mergeCell ref="I17:I23"/>
-    <mergeCell ref="N17:N23"/>
+    <mergeCell ref="O17:O23"/>
     <mergeCell ref="C17:C23"/>
-    <mergeCell ref="O17:O23"/>
+    <mergeCell ref="P17:P23"/>
+    <mergeCell ref="Q17:Q23"/>
+    <mergeCell ref="BR17:BR23"/>
+    <mergeCell ref="R25:R31"/>
+    <mergeCell ref="S25:S31"/>
+    <mergeCell ref="BN17:BN23"/>
+    <mergeCell ref="BO17:BO23"/>
+    <mergeCell ref="P25:P31"/>
+    <mergeCell ref="K17:K23"/>
+    <mergeCell ref="BG17:BG23"/>
+    <mergeCell ref="BH17:BH23"/>
     <mergeCell ref="BI17:BI23"/>
-    <mergeCell ref="P17:P23"/>
-    <mergeCell ref="R17:R23"/>
+    <mergeCell ref="BJ17:BJ23"/>
+    <mergeCell ref="S17:S23"/>
     <mergeCell ref="BS17:BS23"/>
     <mergeCell ref="BK17:BK23"/>
-    <mergeCell ref="Q17:Q23"/>
-    <mergeCell ref="BL17:BL23"/>
-    <mergeCell ref="BM17:BM23"/>
-    <mergeCell ref="AZ17:AZ23"/>
-    <mergeCell ref="AX17:AX23"/>
-    <mergeCell ref="AY17:AY23"/>
-    <mergeCell ref="U17:U23"/>
-    <mergeCell ref="BA17:BA23"/>
-    <mergeCell ref="AL17:AL23"/>
-    <mergeCell ref="AQ17:AQ23"/>
-    <mergeCell ref="AV17:AV23"/>
-    <mergeCell ref="AK17:AK23"/>
-    <mergeCell ref="X17:X23"/>
-    <mergeCell ref="BB17:BB23"/>
-    <mergeCell ref="Z17:Z23"/>
-    <mergeCell ref="AF17:AF23"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="AA17:AA23"/>
-    <mergeCell ref="AB17:AB23"/>
-    <mergeCell ref="V17:V23"/>
-    <mergeCell ref="W17:W23"/>
-    <mergeCell ref="K17:K23"/>
-    <mergeCell ref="L17:L23"/>
-    <mergeCell ref="J17:J23"/>
-    <mergeCell ref="S17:S23"/>
-    <mergeCell ref="T17:T23"/>
-    <mergeCell ref="D17:D23"/>
-    <mergeCell ref="AI17:AI23"/>
-    <mergeCell ref="AI25:AI30"/>
-    <mergeCell ref="BT17:BT23"/>
-    <mergeCell ref="AD17:AD23"/>
-    <mergeCell ref="AE17:AE23"/>
-    <mergeCell ref="AG17:AG23"/>
-    <mergeCell ref="BE17:BE23"/>
-    <mergeCell ref="AR17:AR23"/>
-    <mergeCell ref="AS17:AS23"/>
-    <mergeCell ref="AT17:AT23"/>
-    <mergeCell ref="AU17:AU23"/>
-    <mergeCell ref="AM17:AM23"/>
-    <mergeCell ref="AN17:AN23"/>
-    <mergeCell ref="AO17:AO23"/>
-    <mergeCell ref="AP17:AP23"/>
+    <mergeCell ref="S33:S37"/>
+    <mergeCell ref="BP17:BP23"/>
+    <mergeCell ref="BQ17:BQ23"/>
     <mergeCell ref="AJ17:AJ23"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="BF24:BF30"/>
-    <mergeCell ref="BE33:BE36"/>
-    <mergeCell ref="BE25:BE31"/>
-    <mergeCell ref="AW17:AW23"/>
-    <mergeCell ref="AW25:AW31"/>
-    <mergeCell ref="M17:M23"/>
-    <mergeCell ref="M25:M31"/>
-    <mergeCell ref="AQ25:AQ30"/>
-    <mergeCell ref="AT25:AT30"/>
-    <mergeCell ref="AU25:AU30"/>
-    <mergeCell ref="AL25:AL30"/>
-    <mergeCell ref="AM25:AM30"/>
-    <mergeCell ref="AP25:AP30"/>
-    <mergeCell ref="AH17:AH23"/>
-    <mergeCell ref="AH25:AH30"/>
+    <mergeCell ref="AJ25:AJ30"/>
+    <mergeCell ref="I2:AX4"/>
+    <mergeCell ref="BG2:BJ4"/>
+    <mergeCell ref="BK2:BS4"/>
+    <mergeCell ref="AY2:BE4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>